<commit_message>
Pivot table created perfectly
</commit_message>
<xml_diff>
--- a/CMPM/cmpm_modified.xlsx
+++ b/CMPM/cmpm_modified.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Workings\Revathi\flaskapi\CMPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB960B67-7693-4B18-BE06-AFC388EACF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1F790F-C23B-4156-BB88-08A65A13DC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
+    <pivotCache cacheId="11" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Date Report Generated: 07/31/2024</t>
   </si>
@@ -69,7 +69,7 @@
     <t>Resource ATTUID</t>
   </si>
   <si>
-    <t>Feb</t>
+    <t>Sep</t>
   </si>
   <si>
     <t>Rate</t>
@@ -117,13 +117,19 @@
     <t>Subtotal</t>
   </si>
   <si>
+    <t>(All)</t>
+  </si>
+  <si>
     <t>Row Labels</t>
   </si>
   <si>
+    <t>(blank)</t>
+  </si>
+  <si>
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Sum of Feb</t>
+    <t>Sum of Sep</t>
   </si>
   <si>
     <t>Sum of Total Cost</t>
@@ -162,11 +168,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -187,31 +196,28 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Harishkumar J." refreshedDate="45666.477196180553" createdVersion="6" refreshedVersion="8" minRefreshableVersion="3" recordCount="5" xr:uid="{64594D83-C889-4705-9830-25545AC011B3}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Harishkumar J." refreshedDate="45666.526990046295" createdVersion="6" refreshedVersion="8" minRefreshableVersion="3" recordCount="5" xr:uid="{7671ED09-19F3-4B65-87D1-706911BFBE22}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A9:I14" sheet="Modified Data"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="PMT Title" numFmtId="0">
-      <sharedItems count="5">
-        <s v="Ericsson 1.32 SW Upgrade for cMME PCC 1.32"/>
-        <s v="Ericsson 1.32 SW Upgrade for cMME PCC 1.35"/>
-        <s v="Ericsson 1.32 SW Upgrade for cMME PCC 1.36"/>
-        <s v="Ericsson 1.32 SW Upgrade for cMME PCC 1.37"/>
-        <s v="Subtotal"/>
-      </sharedItems>
+      <sharedItems/>
     </cacheField>
     <cacheField name="Cost Center" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Application" numFmtId="0">
-      <sharedItems containsBlank="1"/>
+      <sharedItems containsBlank="1" count="2">
+        <s v="Network Service Assurance System NSAS"/>
+        <m/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Resource ATTUID" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
-    <cacheField name="Feb" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4" maxValue="16"/>
+    <cacheField name="Sep" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4" maxValue="22"/>
     </cacheField>
     <cacheField name="Rate" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
@@ -220,10 +226,14 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
     </cacheField>
     <cacheField name="Location" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Employee" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -237,104 +247,103 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="5">
   <r>
-    <x v="0"/>
+    <s v="Ericsson 1.32 SW Upgrade for cMME PCC 1.32"/>
     <s v="EY1Z18000"/>
-    <s v="Network Service Assurance System NSAS"/>
+    <x v="0"/>
     <s v="sa8978"/>
     <n v="4"/>
     <m/>
     <n v="0"/>
-    <m/>
-    <m/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
-    <x v="1"/>
+    <s v="Ericsson 1.32 SW Upgrade for cMME PCC 1.35"/>
     <s v="EY1Z18000"/>
-    <s v="Network Service Assurance System NSAS"/>
+    <x v="0"/>
     <s v="sa8981"/>
-    <n v="4"/>
+    <n v="6"/>
     <m/>
     <n v="0"/>
-    <m/>
-    <m/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
-    <x v="2"/>
+    <s v="Ericsson 1.32 SW Upgrade for cMME PCC 1.36"/>
     <s v="EY1Z18000"/>
-    <s v="Network Service Assurance System NSAS"/>
+    <x v="0"/>
     <s v="sa8982"/>
-    <n v="4"/>
+    <n v="6"/>
     <m/>
     <n v="0"/>
-    <m/>
-    <m/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
-    <x v="3"/>
+    <s v="Ericsson 1.32 SW Upgrade for cMME PCC 1.37"/>
     <s v="EY1Z18000"/>
-    <s v="Network Service Assurance System NSAS"/>
+    <x v="0"/>
     <s v="sa8983"/>
-    <n v="4"/>
+    <n v="6"/>
     <m/>
     <n v="0"/>
-    <m/>
-    <m/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
-    <x v="4"/>
+    <s v="Subtotal"/>
     <m/>
+    <x v="1"/>
     <m/>
-    <m/>
-    <n v="16"/>
+    <n v="22"/>
     <m/>
     <n v="0"/>
-    <m/>
-    <m/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BF8B6AB9-7AFF-4EB0-AD1C-565B85D78CB0}" name="SummaryPivotTable" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A7B7F5E5-1823-4BF1-A78F-0A33BB5DC54F}" name="SummaryPivotTable" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="3">
         <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
   </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
+  <rowFields count="2">
+    <field x="7"/>
+    <field x="8"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="3">
     <i>
       <x/>
     </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
+    <i r="1">
+      <x/>
     </i>
     <i t="grand">
       <x/>
@@ -351,8 +360,11 @@
       <x v="1"/>
     </i>
   </colItems>
+  <pageFields count="1">
+    <pageField fld="2" hier="-1"/>
+  </pageFields>
   <dataFields count="2">
-    <dataField name="Sum of Feb" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Sep" fld="4" baseField="0" baseItem="0"/>
     <dataField name="Sum of Total Cost" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -651,92 +663,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D78F936-C5A5-424C-B7AE-FA48B705AB21}">
-  <dimension ref="A3:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD7E6A1-DF45-4C42-B40B-5224084E6F90}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="37.29296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.76171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.05859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.8203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.8203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3">
+        <v>28</v>
+      </c>
+      <c r="B4" s="4">
+        <v>44</v>
+      </c>
+      <c r="C4" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="4">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="3">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="3">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="3">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="3">
-        <v>32</v>
-      </c>
-      <c r="C9" s="3">
+        <v>29</v>
+      </c>
+      <c r="B6" s="4">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4">
         <v>0</v>
       </c>
     </row>
@@ -847,7 +834,7 @@
         <v>20</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G11">
         <f>E11*F11</f>
@@ -868,7 +855,7 @@
         <v>22</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G12">
         <f>E12*F12</f>
@@ -889,7 +876,7 @@
         <v>24</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G13">
         <f>E13*F13</f>
@@ -902,7 +889,7 @@
       </c>
       <c r="E14">
         <f>SUBTOTAL(9,E10:E13)</f>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G14">
         <f>SUBTOTAL(9,G10:G13)</f>

</xml_diff>